<commit_message>
Fully functional app with exe generated and being used.
</commit_message>
<xml_diff>
--- a/Personal Projects/task_timer/Task_Timer.xlsx
+++ b/Personal Projects/task_timer/Task_Timer.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tasks" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Time" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Time" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,277 +414,570 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="20.36328125" bestFit="1" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Tasks</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>Task</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Added_On</t>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Start_Time</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>End_Time</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Total_Seconds</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Add</t>
+          <t>14-Jun-2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Refresh</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T06:53 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>11:27 PM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>11:27 PM</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PDS</t>
+          <t>14-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T06:53 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>11:28 PM</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>11:28 PM</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T07:18 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>test task</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12:19 PM</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>12:19 PM</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PDS</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T07:18 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12:36 PM</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>12:36 PM</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Iovh</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T07:29 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>12:36 PM</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12:36 PM</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Task Timer</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T10:56 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>12:36 PM</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12:37 PM</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Timer App</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Jun 11, 2025 T10:58 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12:40 PM</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12:40 PM</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>B10</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T12:00 AM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12:41 PM</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>12:42 PM</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>New1</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T12:08 AM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>12:43 PM</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>12:43 PM</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>100days</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T12:08 AM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12:43 PM</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>12:43 PM</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T12:09 AM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12:45 PM</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>12:45 PM</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Refresh</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T08:36 AM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>02:19 PM</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>02:19 PM</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Another</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Active</t>
-        </is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>02:23 PM</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>02:23 PM</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Df</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T12:04 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>02:23 PM</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>02:24 PM</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Addqe</t>
+          <t>15-Jun-2025</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Jun 12, 2025 T12:06 PM</t>
-        </is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Task Notes</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>02:50 PM</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>02:51 PM</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>15-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>06:13 PM</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>06:13 PM</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -697,283 +991,63 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="10.90625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.81640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="22.6328125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9.81640625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="9.08984375" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="12.90625" bestFit="1" customWidth="1" min="7" max="7"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Tasks</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>Status</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Duration</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Start_Time</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>End_Time</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Total_Seconds</t>
+          <t>Added_On</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>12-Jun-2025</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Task Timer</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0h:00m</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12:28 AM</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12:28 AM</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>4</v>
+          <t>14-Jun-2025 T11:28 PM</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12-Jun-2025</t>
+          <t>New</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Task Timer</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0h:00m</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>tESTING in the final stages</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>12:31 AM</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>12:31 AM</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>12-Jun-2025</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Refresh</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1h:42m</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>08:36 AM</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>10:19 AM</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>12-Jun-2025</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Refresh</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0h:00m</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10:20 AM</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>10:20 AM</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>12-Jun-2025</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Timer App</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0h:00m</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10:24 AM</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>10:24 AM</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>12-Jun-2025</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Refresh</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0h:00m</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>10:24 AM</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>10:25 AM</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>12-Jun-2025</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>New1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0h:00m</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>we</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>11:30 AM</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>11:30 AM</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>7</v>
+          <t>15-Jun-2025 T12:19 PM</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TimeKeeper-fixed notes capturing default text
</commit_message>
<xml_diff>
--- a/Personal Projects/task_timer/Task_Timer.xlsx
+++ b/Personal Projects/task_timer/Task_Timer.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,7 +965,6 @@
           <t>0h:00m</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
           <t>06:13 PM</t>
@@ -978,6 +977,236 @@
       </c>
       <c r="G17" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12:06 PM</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>12:06 PM</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Test notes</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12:07 PM</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>12:07 PM</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>12:09 PM</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>12:09 PM</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>12:11 PM</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>12:11 PM</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>dfghj</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>12:11 PM</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>12:11 PM</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>12:12 PM</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>12:13 PM</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>16-Jun-2025</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0h:00m</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>12:13 PM</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>12:13 PM</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>